<commit_message>
added default settings to ignore list
</commit_message>
<xml_diff>
--- a/Experiment_Database_backup.xlsx
+++ b/Experiment_Database_backup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11965" windowHeight="4566"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22478" windowHeight="8780"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5558" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6166" uniqueCount="109">
   <si>
     <t>Experiment Database</t>
   </si>
@@ -337,6 +337,15 @@
   </si>
   <si>
     <t>1.30Hz-7cm</t>
+  </si>
+  <si>
+    <t>6/27/2016</t>
+  </si>
+  <si>
+    <t>new rails and bearings</t>
+  </si>
+  <si>
+    <t>6/29/2016</t>
   </si>
 </sst>
 </file>
@@ -778,11 +787,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W669"/>
+  <dimension ref="A1:W737"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A649" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I674" sqref="I674"/>
+      <pane ySplit="2" topLeftCell="A718" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A737" sqref="A737"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
@@ -808,8 +817,8 @@
     <col min="21" max="21" width="13.09765625" style="15" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.19921875" style="15" customWidth="1"/>
     <col min="23" max="23" width="23.69921875" style="15" bestFit="1" customWidth="1"/>
-    <col min="24" max="144" width="9.09765625" style="1" customWidth="1"/>
-    <col min="145" max="16384" width="9.09765625" style="1"/>
+    <col min="24" max="157" width="9.09765625" style="1" customWidth="1"/>
+    <col min="158" max="16384" width="9.09765625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -5303,7 +5312,7 @@
         <v>7.72</v>
       </c>
       <c r="R67" s="4">
-        <f t="shared" ref="R67:R80" si="2">AVERAGE(N67:Q67)</f>
+        <f t="shared" ref="R67:R98" si="2">AVERAGE(N67:Q67)</f>
         <v>7.7724999999999991</v>
       </c>
       <c r="S67" s="15" t="s">
@@ -45317,7 +45326,4618 @@
       <c r="V669" s="15">
         <v>5</v>
       </c>
-      <c r="W669"/>
+    </row>
+    <row r="670" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A670" s="15">
+        <v>716</v>
+      </c>
+      <c r="B670" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C670" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D670" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E670" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F670" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G670" s="15">
+        <v>10</v>
+      </c>
+      <c r="H670" s="15">
+        <v>22</v>
+      </c>
+      <c r="I670" s="15">
+        <v>20</v>
+      </c>
+      <c r="J670" s="15">
+        <v>60</v>
+      </c>
+      <c r="K670" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L670" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N670" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="O670" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="P670" s="15">
+        <v>3.48</v>
+      </c>
+      <c r="Q670" s="15">
+        <v>3.49</v>
+      </c>
+      <c r="R670" s="15">
+        <v>3.49</v>
+      </c>
+      <c r="S670" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T670" s="15">
+        <v>15</v>
+      </c>
+      <c r="U670" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V670" s="15">
+        <v>5</v>
+      </c>
+      <c r="W670" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="671" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A671" s="15">
+        <v>717</v>
+      </c>
+      <c r="B671" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C671" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D671" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E671" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F671" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G671" s="15">
+        <v>10</v>
+      </c>
+      <c r="H671" s="15">
+        <v>22</v>
+      </c>
+      <c r="I671" s="15">
+        <v>20</v>
+      </c>
+      <c r="J671" s="15">
+        <v>60</v>
+      </c>
+      <c r="K671" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L671" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N671" s="15">
+        <v>6.45</v>
+      </c>
+      <c r="O671" s="15">
+        <v>6.4</v>
+      </c>
+      <c r="P671" s="15">
+        <v>6.4</v>
+      </c>
+      <c r="Q671" s="15">
+        <v>6.36</v>
+      </c>
+      <c r="R671" s="15">
+        <v>6.4</v>
+      </c>
+      <c r="S671" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T671" s="15">
+        <v>15</v>
+      </c>
+      <c r="U671" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V671" s="15">
+        <v>5</v>
+      </c>
+      <c r="W671" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="672" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A672" s="15">
+        <v>718</v>
+      </c>
+      <c r="B672" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C672" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D672" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E672" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F672" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G672" s="15">
+        <v>10</v>
+      </c>
+      <c r="H672" s="15">
+        <v>22</v>
+      </c>
+      <c r="I672" s="15">
+        <v>20</v>
+      </c>
+      <c r="J672" s="15">
+        <v>60</v>
+      </c>
+      <c r="K672" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L672" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N672" s="15">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="O672" s="15">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="P672" s="15">
+        <v>7.97</v>
+      </c>
+      <c r="Q672" s="15">
+        <v>8.02</v>
+      </c>
+      <c r="R672" s="15">
+        <v>8.06</v>
+      </c>
+      <c r="S672" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T672" s="15">
+        <v>15</v>
+      </c>
+      <c r="U672" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V672" s="15">
+        <v>5</v>
+      </c>
+      <c r="W672" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="673" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A673" s="15">
+        <v>719</v>
+      </c>
+      <c r="B673" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C673" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D673" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E673" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F673" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G673" s="15">
+        <v>10</v>
+      </c>
+      <c r="H673" s="15">
+        <v>22</v>
+      </c>
+      <c r="I673" s="15">
+        <v>20</v>
+      </c>
+      <c r="J673" s="15">
+        <v>60</v>
+      </c>
+      <c r="K673" s="15">
+        <v>4</v>
+      </c>
+      <c r="L673" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N673" s="15">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="O673" s="15">
+        <v>8.35</v>
+      </c>
+      <c r="P673" s="15">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="Q673" s="15">
+        <v>8.33</v>
+      </c>
+      <c r="R673" s="15">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="S673" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T673" s="15">
+        <v>15</v>
+      </c>
+      <c r="U673" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V673" s="15">
+        <v>5</v>
+      </c>
+      <c r="W673" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="674" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A674" s="15">
+        <v>720</v>
+      </c>
+      <c r="B674" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C674" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D674" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E674" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F674" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G674" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H674" s="15">
+        <v>22</v>
+      </c>
+      <c r="I674" s="15">
+        <v>20</v>
+      </c>
+      <c r="J674" s="15">
+        <v>60</v>
+      </c>
+      <c r="K674" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L674" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N674" s="15">
+        <v>4.29</v>
+      </c>
+      <c r="O674" s="15">
+        <v>4.3</v>
+      </c>
+      <c r="P674" s="15">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="Q674" s="15">
+        <v>4.3</v>
+      </c>
+      <c r="R674" s="15">
+        <v>4.3</v>
+      </c>
+      <c r="S674" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T674" s="15">
+        <v>15</v>
+      </c>
+      <c r="U674" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V674" s="15">
+        <v>5</v>
+      </c>
+      <c r="W674" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="675" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A675" s="15">
+        <v>721</v>
+      </c>
+      <c r="B675" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C675" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D675" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E675" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F675" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G675" s="15">
+        <v>20</v>
+      </c>
+      <c r="H675" s="15">
+        <v>22</v>
+      </c>
+      <c r="I675" s="15">
+        <v>20</v>
+      </c>
+      <c r="J675" s="15">
+        <v>60</v>
+      </c>
+      <c r="K675" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L675" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N675" s="15">
+        <v>5.81</v>
+      </c>
+      <c r="O675" s="15">
+        <v>5.8</v>
+      </c>
+      <c r="P675" s="15">
+        <v>5.8</v>
+      </c>
+      <c r="Q675" s="15">
+        <v>5.8</v>
+      </c>
+      <c r="R675" s="15">
+        <v>5.8</v>
+      </c>
+      <c r="S675" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T675" s="15">
+        <v>15</v>
+      </c>
+      <c r="U675" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V675" s="15">
+        <v>5</v>
+      </c>
+      <c r="W675" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="676" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A676" s="15">
+        <v>722</v>
+      </c>
+      <c r="B676" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C676" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D676" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E676" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F676" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G676" s="15">
+        <v>30</v>
+      </c>
+      <c r="H676" s="15">
+        <v>22</v>
+      </c>
+      <c r="I676" s="15">
+        <v>20</v>
+      </c>
+      <c r="J676" s="15">
+        <v>60</v>
+      </c>
+      <c r="K676" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L676" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N676" s="15">
+        <v>7.46</v>
+      </c>
+      <c r="O676" s="15">
+        <v>7.45</v>
+      </c>
+      <c r="P676" s="15">
+        <v>7.46</v>
+      </c>
+      <c r="Q676" s="15">
+        <v>7.49</v>
+      </c>
+      <c r="R676" s="15">
+        <v>7.46</v>
+      </c>
+      <c r="S676" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T676" s="15">
+        <v>15</v>
+      </c>
+      <c r="U676" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V676" s="15">
+        <v>5</v>
+      </c>
+      <c r="W676" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="677" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A677" s="15">
+        <v>723</v>
+      </c>
+      <c r="B677" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C677" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D677" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E677" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F677" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G677" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H677" s="15">
+        <v>22</v>
+      </c>
+      <c r="I677" s="15">
+        <v>20</v>
+      </c>
+      <c r="J677" s="15">
+        <v>60</v>
+      </c>
+      <c r="K677" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L677" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N677" s="15">
+        <v>7.57</v>
+      </c>
+      <c r="O677" s="15">
+        <v>7.61</v>
+      </c>
+      <c r="P677" s="15">
+        <v>7.61</v>
+      </c>
+      <c r="Q677" s="15">
+        <v>7.58</v>
+      </c>
+      <c r="R677" s="15">
+        <v>7.59</v>
+      </c>
+      <c r="S677" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T677" s="15">
+        <v>15</v>
+      </c>
+      <c r="U677" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V677" s="15">
+        <v>5</v>
+      </c>
+      <c r="W677" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="678" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A678" s="15">
+        <v>724</v>
+      </c>
+      <c r="B678" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C678" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D678" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E678" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F678" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G678" s="15">
+        <v>20</v>
+      </c>
+      <c r="H678" s="15">
+        <v>22</v>
+      </c>
+      <c r="I678" s="15">
+        <v>20</v>
+      </c>
+      <c r="J678" s="15">
+        <v>60</v>
+      </c>
+      <c r="K678" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L678" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N678" s="15">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="O678" s="15">
+        <v>8.86</v>
+      </c>
+      <c r="P678" s="15">
+        <v>8.86</v>
+      </c>
+      <c r="Q678" s="15">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="R678" s="15">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="S678" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T678" s="15">
+        <v>15</v>
+      </c>
+      <c r="U678" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V678" s="15">
+        <v>5</v>
+      </c>
+      <c r="W678" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="679" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A679" s="15">
+        <v>725</v>
+      </c>
+      <c r="B679" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C679" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D679" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E679" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F679" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G679" s="15">
+        <v>30</v>
+      </c>
+      <c r="H679" s="15">
+        <v>22</v>
+      </c>
+      <c r="I679" s="15">
+        <v>20</v>
+      </c>
+      <c r="J679" s="15">
+        <v>60</v>
+      </c>
+      <c r="K679" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L679" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N679" s="15">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="O679" s="15">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="P679" s="15">
+        <v>9.18</v>
+      </c>
+      <c r="Q679" s="15">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="R679" s="15">
+        <v>9.16</v>
+      </c>
+      <c r="S679" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T679" s="15">
+        <v>15</v>
+      </c>
+      <c r="U679" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V679" s="15">
+        <v>5</v>
+      </c>
+      <c r="W679" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="680" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A680" s="15">
+        <v>726</v>
+      </c>
+      <c r="B680" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C680" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D680" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E680" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F680" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G680" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H680" s="15">
+        <v>22</v>
+      </c>
+      <c r="I680" s="15">
+        <v>20</v>
+      </c>
+      <c r="J680" s="15">
+        <v>60</v>
+      </c>
+      <c r="K680" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L680" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N680" s="15">
+        <v>8.59</v>
+      </c>
+      <c r="O680" s="15">
+        <v>8.59</v>
+      </c>
+      <c r="P680" s="15">
+        <v>8.57</v>
+      </c>
+      <c r="Q680" s="15">
+        <v>8.56</v>
+      </c>
+      <c r="R680" s="15">
+        <v>8.58</v>
+      </c>
+      <c r="S680" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T680" s="15">
+        <v>15</v>
+      </c>
+      <c r="U680" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V680" s="15">
+        <v>5</v>
+      </c>
+      <c r="W680" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="681" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A681" s="15">
+        <v>727</v>
+      </c>
+      <c r="B681" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C681" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D681" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E681" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F681" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G681" s="15">
+        <v>20</v>
+      </c>
+      <c r="H681" s="15">
+        <v>22</v>
+      </c>
+      <c r="I681" s="15">
+        <v>20</v>
+      </c>
+      <c r="J681" s="15">
+        <v>60</v>
+      </c>
+      <c r="K681" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L681" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N681" s="15">
+        <v>7.71</v>
+      </c>
+      <c r="O681" s="15">
+        <v>7.69</v>
+      </c>
+      <c r="P681" s="15">
+        <v>7.69</v>
+      </c>
+      <c r="Q681" s="15">
+        <v>7.7</v>
+      </c>
+      <c r="R681" s="15">
+        <v>7.7</v>
+      </c>
+      <c r="S681" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T681" s="15">
+        <v>15</v>
+      </c>
+      <c r="U681" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V681" s="15">
+        <v>5</v>
+      </c>
+      <c r="W681" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="682" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A682" s="15">
+        <v>728</v>
+      </c>
+      <c r="B682" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C682" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D682" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E682" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F682" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G682" s="15">
+        <v>30</v>
+      </c>
+      <c r="H682" s="15">
+        <v>22</v>
+      </c>
+      <c r="I682" s="15">
+        <v>20</v>
+      </c>
+      <c r="J682" s="15">
+        <v>60</v>
+      </c>
+      <c r="K682" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L682" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N682" s="15">
+        <v>6.26</v>
+      </c>
+      <c r="O682" s="15">
+        <v>6.26</v>
+      </c>
+      <c r="P682" s="15">
+        <v>6.28</v>
+      </c>
+      <c r="Q682" s="15">
+        <v>6.3</v>
+      </c>
+      <c r="R682" s="15">
+        <v>6.28</v>
+      </c>
+      <c r="S682" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T682" s="15">
+        <v>15</v>
+      </c>
+      <c r="U682" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V682" s="15">
+        <v>5</v>
+      </c>
+      <c r="W682" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="683" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A683" s="15">
+        <v>729</v>
+      </c>
+      <c r="B683" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C683" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D683" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E683" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F683" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G683" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H683" s="15">
+        <v>22</v>
+      </c>
+      <c r="I683" s="15">
+        <v>20</v>
+      </c>
+      <c r="J683" s="15">
+        <v>60</v>
+      </c>
+      <c r="K683" s="15">
+        <v>4</v>
+      </c>
+      <c r="L683" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N683" s="15">
+        <v>8.64</v>
+      </c>
+      <c r="O683" s="15">
+        <v>8.59</v>
+      </c>
+      <c r="P683" s="15">
+        <v>8.58</v>
+      </c>
+      <c r="Q683" s="15">
+        <v>8.59</v>
+      </c>
+      <c r="R683" s="15">
+        <v>8.6</v>
+      </c>
+      <c r="S683" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T683" s="15">
+        <v>15</v>
+      </c>
+      <c r="U683" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V683" s="15">
+        <v>5</v>
+      </c>
+      <c r="W683" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="684" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A684" s="15">
+        <v>730</v>
+      </c>
+      <c r="B684" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C684" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D684" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E684" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F684" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G684" s="15">
+        <v>20</v>
+      </c>
+      <c r="H684" s="15">
+        <v>22</v>
+      </c>
+      <c r="I684" s="15">
+        <v>20</v>
+      </c>
+      <c r="J684" s="15">
+        <v>60</v>
+      </c>
+      <c r="K684" s="15">
+        <v>4</v>
+      </c>
+      <c r="L684" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N684" s="15">
+        <v>7.3</v>
+      </c>
+      <c r="O684" s="15">
+        <v>7.29</v>
+      </c>
+      <c r="P684" s="15">
+        <v>7.32</v>
+      </c>
+      <c r="Q684" s="15">
+        <v>7.34</v>
+      </c>
+      <c r="R684" s="15">
+        <v>7.31</v>
+      </c>
+      <c r="S684" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T684" s="15">
+        <v>15</v>
+      </c>
+      <c r="U684" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V684" s="15">
+        <v>5</v>
+      </c>
+      <c r="W684" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="685" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A685" s="15">
+        <v>731</v>
+      </c>
+      <c r="B685" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C685" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D685" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E685" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F685" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G685" s="15">
+        <v>30</v>
+      </c>
+      <c r="H685" s="15">
+        <v>22</v>
+      </c>
+      <c r="I685" s="15">
+        <v>20</v>
+      </c>
+      <c r="J685" s="15">
+        <v>60</v>
+      </c>
+      <c r="K685" s="15">
+        <v>4</v>
+      </c>
+      <c r="L685" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N685" s="15">
+        <v>5.75</v>
+      </c>
+      <c r="O685" s="15">
+        <v>5.75</v>
+      </c>
+      <c r="P685" s="15">
+        <v>5.76</v>
+      </c>
+      <c r="Q685" s="15">
+        <v>5.78</v>
+      </c>
+      <c r="R685" s="15">
+        <v>5.76</v>
+      </c>
+      <c r="S685" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T685" s="15">
+        <v>15</v>
+      </c>
+      <c r="U685" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V685" s="15">
+        <v>5</v>
+      </c>
+      <c r="W685" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="686" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A686" s="15">
+        <v>732</v>
+      </c>
+      <c r="B686" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C686" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D686" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E686" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F686" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G686" s="15">
+        <v>10</v>
+      </c>
+      <c r="H686" s="15">
+        <v>22</v>
+      </c>
+      <c r="I686" s="15">
+        <v>20</v>
+      </c>
+      <c r="J686" s="15">
+        <v>45</v>
+      </c>
+      <c r="K686" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L686" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N686" s="15">
+        <v>1.71</v>
+      </c>
+      <c r="O686" s="15">
+        <v>1.78</v>
+      </c>
+      <c r="P686" s="15">
+        <v>1.81</v>
+      </c>
+      <c r="Q686" s="15">
+        <v>1.82</v>
+      </c>
+      <c r="R686" s="15">
+        <v>1.78</v>
+      </c>
+      <c r="S686" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T686" s="15">
+        <v>15</v>
+      </c>
+      <c r="U686" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V686" s="15">
+        <v>5</v>
+      </c>
+      <c r="W686" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="687" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A687" s="15">
+        <v>733</v>
+      </c>
+      <c r="B687" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C687" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D687" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E687" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F687" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G687" s="15">
+        <v>10</v>
+      </c>
+      <c r="H687" s="15">
+        <v>22</v>
+      </c>
+      <c r="I687" s="15">
+        <v>20</v>
+      </c>
+      <c r="J687" s="15">
+        <v>45</v>
+      </c>
+      <c r="K687" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L687" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N687" s="15">
+        <v>4.7</v>
+      </c>
+      <c r="O687" s="15">
+        <v>4.72</v>
+      </c>
+      <c r="P687" s="15">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="Q687" s="15">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="R687" s="15">
+        <v>4.72</v>
+      </c>
+      <c r="S687" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T687" s="15">
+        <v>15</v>
+      </c>
+      <c r="U687" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V687" s="15">
+        <v>5</v>
+      </c>
+      <c r="W687" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="688" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A688" s="15">
+        <v>734</v>
+      </c>
+      <c r="B688" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C688" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D688" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E688" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F688" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G688" s="15">
+        <v>10</v>
+      </c>
+      <c r="H688" s="15">
+        <v>22</v>
+      </c>
+      <c r="I688" s="15">
+        <v>20</v>
+      </c>
+      <c r="J688" s="15">
+        <v>45</v>
+      </c>
+      <c r="K688" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L688" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N688" s="15">
+        <v>6.67</v>
+      </c>
+      <c r="O688" s="15">
+        <v>6.68</v>
+      </c>
+      <c r="P688" s="15">
+        <v>6.71</v>
+      </c>
+      <c r="Q688" s="15">
+        <v>6.84</v>
+      </c>
+      <c r="R688" s="15">
+        <v>6.72</v>
+      </c>
+      <c r="S688" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T688" s="15">
+        <v>15</v>
+      </c>
+      <c r="U688" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V688" s="15">
+        <v>5</v>
+      </c>
+      <c r="W688" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="689" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A689" s="15">
+        <v>735</v>
+      </c>
+      <c r="B689" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C689" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D689" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E689" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F689" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G689" s="15">
+        <v>10</v>
+      </c>
+      <c r="H689" s="15">
+        <v>22</v>
+      </c>
+      <c r="I689" s="15">
+        <v>20</v>
+      </c>
+      <c r="J689" s="15">
+        <v>45</v>
+      </c>
+      <c r="K689" s="15">
+        <v>4</v>
+      </c>
+      <c r="L689" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N689" s="15">
+        <v>7.17</v>
+      </c>
+      <c r="O689" s="15">
+        <v>7.16</v>
+      </c>
+      <c r="P689" s="15">
+        <v>7.23</v>
+      </c>
+      <c r="Q689" s="15">
+        <v>7.22</v>
+      </c>
+      <c r="R689" s="15">
+        <v>7.2</v>
+      </c>
+      <c r="S689" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T689" s="15">
+        <v>15</v>
+      </c>
+      <c r="U689" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V689" s="15">
+        <v>5</v>
+      </c>
+      <c r="W689" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="690" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A690" s="15">
+        <v>736</v>
+      </c>
+      <c r="B690" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C690" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D690" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E690" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F690" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G690" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H690" s="15">
+        <v>22</v>
+      </c>
+      <c r="I690" s="15">
+        <v>20</v>
+      </c>
+      <c r="J690" s="15">
+        <v>45</v>
+      </c>
+      <c r="K690" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L690" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N690" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O690" s="15">
+        <v>2.31</v>
+      </c>
+      <c r="P690" s="15">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="Q690" s="15">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="R690" s="15">
+        <v>2.31</v>
+      </c>
+      <c r="S690" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T690" s="15">
+        <v>15</v>
+      </c>
+      <c r="U690" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V690" s="15">
+        <v>5</v>
+      </c>
+      <c r="W690" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="691" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A691" s="15">
+        <v>737</v>
+      </c>
+      <c r="B691" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C691" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D691" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E691" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F691" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G691" s="15">
+        <v>20</v>
+      </c>
+      <c r="H691" s="15">
+        <v>22</v>
+      </c>
+      <c r="I691" s="15">
+        <v>20</v>
+      </c>
+      <c r="J691" s="15">
+        <v>45</v>
+      </c>
+      <c r="K691" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L691" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N691" s="15">
+        <v>2.92</v>
+      </c>
+      <c r="O691" s="15">
+        <v>2.92</v>
+      </c>
+      <c r="P691" s="15">
+        <v>2.92</v>
+      </c>
+      <c r="Q691" s="15">
+        <v>2.92</v>
+      </c>
+      <c r="R691" s="15">
+        <v>2.92</v>
+      </c>
+      <c r="S691" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T691" s="15">
+        <v>15</v>
+      </c>
+      <c r="U691" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V691" s="15">
+        <v>5</v>
+      </c>
+      <c r="W691" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="692" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A692" s="15">
+        <v>738</v>
+      </c>
+      <c r="B692" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C692" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D692" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E692" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F692" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G692" s="15">
+        <v>30</v>
+      </c>
+      <c r="H692" s="15">
+        <v>22</v>
+      </c>
+      <c r="I692" s="15">
+        <v>20</v>
+      </c>
+      <c r="J692" s="15">
+        <v>45</v>
+      </c>
+      <c r="K692" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L692" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N692" s="15">
+        <v>3.38</v>
+      </c>
+      <c r="O692" s="15">
+        <v>3.37</v>
+      </c>
+      <c r="P692" s="15">
+        <v>3.35</v>
+      </c>
+      <c r="Q692" s="15">
+        <v>3.34</v>
+      </c>
+      <c r="R692" s="15">
+        <v>3.36</v>
+      </c>
+      <c r="S692" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T692" s="15">
+        <v>15</v>
+      </c>
+      <c r="U692" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V692" s="15">
+        <v>5</v>
+      </c>
+      <c r="W692" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="693" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A693" s="15">
+        <v>739</v>
+      </c>
+      <c r="B693" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C693" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D693" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E693" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F693" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G693" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H693" s="15">
+        <v>22</v>
+      </c>
+      <c r="I693" s="15">
+        <v>20</v>
+      </c>
+      <c r="J693" s="15">
+        <v>45</v>
+      </c>
+      <c r="K693" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L693" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N693" s="15">
+        <v>5.69</v>
+      </c>
+      <c r="O693" s="15">
+        <v>5.69</v>
+      </c>
+      <c r="P693" s="15">
+        <v>5.66</v>
+      </c>
+      <c r="Q693" s="15">
+        <v>5.71</v>
+      </c>
+      <c r="R693" s="15">
+        <v>5.69</v>
+      </c>
+      <c r="S693" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T693" s="15">
+        <v>15</v>
+      </c>
+      <c r="U693" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V693" s="15">
+        <v>5</v>
+      </c>
+      <c r="W693" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="694" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A694" s="15">
+        <v>740</v>
+      </c>
+      <c r="B694" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C694" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D694" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E694" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F694" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G694" s="15">
+        <v>20</v>
+      </c>
+      <c r="H694" s="15">
+        <v>22</v>
+      </c>
+      <c r="I694" s="15">
+        <v>20</v>
+      </c>
+      <c r="J694" s="15">
+        <v>45</v>
+      </c>
+      <c r="K694" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L694" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N694" s="15">
+        <v>7.52</v>
+      </c>
+      <c r="O694" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="P694" s="15">
+        <v>7.52</v>
+      </c>
+      <c r="Q694" s="15">
+        <v>7.51</v>
+      </c>
+      <c r="R694" s="15">
+        <v>7.51</v>
+      </c>
+      <c r="S694" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T694" s="15">
+        <v>15</v>
+      </c>
+      <c r="U694" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V694" s="15">
+        <v>5</v>
+      </c>
+      <c r="W694" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="695" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A695" s="15">
+        <v>741</v>
+      </c>
+      <c r="B695" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C695" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D695" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E695" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F695" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G695" s="15">
+        <v>30</v>
+      </c>
+      <c r="H695" s="15">
+        <v>22</v>
+      </c>
+      <c r="I695" s="15">
+        <v>20</v>
+      </c>
+      <c r="J695" s="15">
+        <v>45</v>
+      </c>
+      <c r="K695" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L695" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N695" s="15">
+        <v>9.01</v>
+      </c>
+      <c r="O695" s="15">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="P695" s="15">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="Q695" s="15">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="R695" s="15">
+        <v>9.01</v>
+      </c>
+      <c r="S695" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T695" s="15">
+        <v>15</v>
+      </c>
+      <c r="U695" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V695" s="15">
+        <v>5</v>
+      </c>
+      <c r="W695" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="696" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A696" s="15">
+        <v>742</v>
+      </c>
+      <c r="B696" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C696" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D696" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E696" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F696" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G696" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H696" s="15">
+        <v>22</v>
+      </c>
+      <c r="I696" s="15">
+        <v>20</v>
+      </c>
+      <c r="J696" s="15">
+        <v>45</v>
+      </c>
+      <c r="K696" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L696" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N696" s="15">
+        <v>7.56</v>
+      </c>
+      <c r="O696" s="15">
+        <v>7.54</v>
+      </c>
+      <c r="P696" s="15">
+        <v>7.51</v>
+      </c>
+      <c r="Q696" s="15">
+        <v>7.48</v>
+      </c>
+      <c r="R696" s="15">
+        <v>7.52</v>
+      </c>
+      <c r="S696" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T696" s="15">
+        <v>15</v>
+      </c>
+      <c r="U696" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V696" s="15">
+        <v>5</v>
+      </c>
+      <c r="W696" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="697" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A697" s="15">
+        <v>743</v>
+      </c>
+      <c r="B697" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C697" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D697" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E697" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F697" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G697" s="15">
+        <v>20</v>
+      </c>
+      <c r="H697" s="15">
+        <v>22</v>
+      </c>
+      <c r="I697" s="15">
+        <v>20</v>
+      </c>
+      <c r="J697" s="15">
+        <v>45</v>
+      </c>
+      <c r="K697" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L697" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N697" s="15">
+        <v>7.64</v>
+      </c>
+      <c r="O697" s="15">
+        <v>7.64</v>
+      </c>
+      <c r="P697" s="15">
+        <v>7.63</v>
+      </c>
+      <c r="Q697" s="15">
+        <v>7.59</v>
+      </c>
+      <c r="R697" s="15">
+        <v>7.62</v>
+      </c>
+      <c r="S697" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T697" s="15">
+        <v>15</v>
+      </c>
+      <c r="U697" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V697" s="15">
+        <v>5</v>
+      </c>
+      <c r="W697" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="698" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A698" s="15">
+        <v>744</v>
+      </c>
+      <c r="B698" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C698" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D698" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E698" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F698" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G698" s="15">
+        <v>30</v>
+      </c>
+      <c r="H698" s="15">
+        <v>22</v>
+      </c>
+      <c r="I698" s="15">
+        <v>20</v>
+      </c>
+      <c r="J698" s="15">
+        <v>45</v>
+      </c>
+      <c r="K698" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L698" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N698" s="15">
+        <v>6.88</v>
+      </c>
+      <c r="O698" s="15">
+        <v>6.91</v>
+      </c>
+      <c r="P698" s="15">
+        <v>6.89</v>
+      </c>
+      <c r="Q698" s="15">
+        <v>6.86</v>
+      </c>
+      <c r="R698" s="15">
+        <v>6.88</v>
+      </c>
+      <c r="S698" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T698" s="15">
+        <v>15</v>
+      </c>
+      <c r="U698" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V698" s="15">
+        <v>5</v>
+      </c>
+      <c r="W698" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="699" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A699" s="15">
+        <v>745</v>
+      </c>
+      <c r="B699" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C699" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D699" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E699" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F699" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G699" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H699" s="15">
+        <v>22</v>
+      </c>
+      <c r="I699" s="15">
+        <v>20</v>
+      </c>
+      <c r="J699" s="15">
+        <v>45</v>
+      </c>
+      <c r="K699" s="15">
+        <v>4</v>
+      </c>
+      <c r="L699" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N699" s="15">
+        <v>7.82</v>
+      </c>
+      <c r="O699" s="15">
+        <v>7.81</v>
+      </c>
+      <c r="P699" s="15">
+        <v>7.84</v>
+      </c>
+      <c r="Q699" s="15">
+        <v>7.88</v>
+      </c>
+      <c r="R699" s="15">
+        <v>7.84</v>
+      </c>
+      <c r="S699" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T699" s="15">
+        <v>15</v>
+      </c>
+      <c r="U699" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V699" s="15">
+        <v>5</v>
+      </c>
+      <c r="W699" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="700" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A700" s="15">
+        <v>746</v>
+      </c>
+      <c r="B700" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C700" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D700" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E700" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F700" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G700" s="15">
+        <v>20</v>
+      </c>
+      <c r="H700" s="15">
+        <v>22</v>
+      </c>
+      <c r="I700" s="15">
+        <v>20</v>
+      </c>
+      <c r="J700" s="15">
+        <v>45</v>
+      </c>
+      <c r="K700" s="15">
+        <v>4</v>
+      </c>
+      <c r="L700" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N700" s="15">
+        <v>7.36</v>
+      </c>
+      <c r="O700" s="15">
+        <v>7.35</v>
+      </c>
+      <c r="P700" s="15">
+        <v>7.36</v>
+      </c>
+      <c r="Q700" s="15">
+        <v>7.36</v>
+      </c>
+      <c r="R700" s="15">
+        <v>7.36</v>
+      </c>
+      <c r="S700" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T700" s="15">
+        <v>15</v>
+      </c>
+      <c r="U700" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V700" s="15">
+        <v>5</v>
+      </c>
+      <c r="W700" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="701" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A701" s="15">
+        <v>747</v>
+      </c>
+      <c r="B701" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C701" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D701" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E701" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F701" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G701" s="15">
+        <v>30</v>
+      </c>
+      <c r="H701" s="15">
+        <v>22</v>
+      </c>
+      <c r="I701" s="15">
+        <v>20</v>
+      </c>
+      <c r="J701" s="15">
+        <v>45</v>
+      </c>
+      <c r="K701" s="15">
+        <v>4</v>
+      </c>
+      <c r="L701" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N701" s="15">
+        <v>6.23</v>
+      </c>
+      <c r="O701" s="15">
+        <v>6.25</v>
+      </c>
+      <c r="P701" s="15">
+        <v>6.27</v>
+      </c>
+      <c r="Q701" s="15">
+        <v>6.24</v>
+      </c>
+      <c r="R701" s="15">
+        <v>6.25</v>
+      </c>
+      <c r="S701" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T701" s="15">
+        <v>15</v>
+      </c>
+      <c r="U701" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V701" s="15">
+        <v>5</v>
+      </c>
+      <c r="W701" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="702" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A702" s="15">
+        <v>748</v>
+      </c>
+      <c r="B702" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C702" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D702" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E702" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F702" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G702" s="15">
+        <v>10</v>
+      </c>
+      <c r="H702" s="15">
+        <v>22</v>
+      </c>
+      <c r="I702" s="15">
+        <v>20</v>
+      </c>
+      <c r="J702" s="15">
+        <v>35</v>
+      </c>
+      <c r="K702" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L702" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N702" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="O702" s="15">
+        <v>0.91</v>
+      </c>
+      <c r="P702" s="15">
+        <v>0.92</v>
+      </c>
+      <c r="Q702" s="15">
+        <v>0.94</v>
+      </c>
+      <c r="R702" s="15">
+        <v>0.92</v>
+      </c>
+      <c r="S702" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T702" s="15">
+        <v>15</v>
+      </c>
+      <c r="U702" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V702" s="15">
+        <v>5</v>
+      </c>
+      <c r="W702" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="703" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A703" s="15">
+        <v>749</v>
+      </c>
+      <c r="B703" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C703" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D703" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E703" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F703" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G703" s="15">
+        <v>10</v>
+      </c>
+      <c r="H703" s="15">
+        <v>22</v>
+      </c>
+      <c r="I703" s="15">
+        <v>20</v>
+      </c>
+      <c r="J703" s="15">
+        <v>35</v>
+      </c>
+      <c r="K703" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L703" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N703" s="15">
+        <v>3.06</v>
+      </c>
+      <c r="O703" s="15">
+        <v>3.05</v>
+      </c>
+      <c r="P703" s="15">
+        <v>3.06</v>
+      </c>
+      <c r="Q703" s="15">
+        <v>3.08</v>
+      </c>
+      <c r="R703" s="15">
+        <v>3.06</v>
+      </c>
+      <c r="S703" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T703" s="15">
+        <v>15</v>
+      </c>
+      <c r="U703" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V703" s="15">
+        <v>5</v>
+      </c>
+      <c r="W703" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="704" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A704" s="15">
+        <v>750</v>
+      </c>
+      <c r="B704" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C704" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D704" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E704" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F704" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G704" s="15">
+        <v>10</v>
+      </c>
+      <c r="H704" s="15">
+        <v>22</v>
+      </c>
+      <c r="I704" s="15">
+        <v>20</v>
+      </c>
+      <c r="J704" s="15">
+        <v>35</v>
+      </c>
+      <c r="K704" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L704" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N704" s="15">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="O704" s="15">
+        <v>5</v>
+      </c>
+      <c r="P704" s="15">
+        <v>4.91</v>
+      </c>
+      <c r="Q704" s="15">
+        <v>5.03</v>
+      </c>
+      <c r="R704" s="15">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="S704" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T704" s="15">
+        <v>15</v>
+      </c>
+      <c r="U704" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V704" s="15">
+        <v>5</v>
+      </c>
+      <c r="W704" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="705" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A705" s="15">
+        <v>751</v>
+      </c>
+      <c r="B705" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C705" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D705" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E705" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F705" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G705" s="15">
+        <v>10</v>
+      </c>
+      <c r="H705" s="15">
+        <v>22</v>
+      </c>
+      <c r="I705" s="15">
+        <v>20</v>
+      </c>
+      <c r="J705" s="15">
+        <v>35</v>
+      </c>
+      <c r="K705" s="15">
+        <v>4</v>
+      </c>
+      <c r="L705" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N705" s="15">
+        <v>5.45</v>
+      </c>
+      <c r="O705" s="15">
+        <v>5.41</v>
+      </c>
+      <c r="P705" s="15">
+        <v>5.53</v>
+      </c>
+      <c r="Q705" s="15">
+        <v>5.5</v>
+      </c>
+      <c r="R705" s="15">
+        <v>5.47</v>
+      </c>
+      <c r="S705" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T705" s="15">
+        <v>15</v>
+      </c>
+      <c r="U705" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V705" s="15">
+        <v>5</v>
+      </c>
+      <c r="W705" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="706" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A706" s="15">
+        <v>752</v>
+      </c>
+      <c r="B706" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C706" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D706" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E706" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F706" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G706" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H706" s="15">
+        <v>22</v>
+      </c>
+      <c r="I706" s="15">
+        <v>20</v>
+      </c>
+      <c r="J706" s="15">
+        <v>35</v>
+      </c>
+      <c r="K706" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L706" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N706" s="15">
+        <v>1.06</v>
+      </c>
+      <c r="O706" s="15">
+        <v>1.08</v>
+      </c>
+      <c r="P706" s="15">
+        <v>1.07</v>
+      </c>
+      <c r="Q706" s="15">
+        <v>1.06</v>
+      </c>
+      <c r="R706" s="15">
+        <v>1.07</v>
+      </c>
+      <c r="S706" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T706" s="15">
+        <v>15</v>
+      </c>
+      <c r="U706" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V706" s="15">
+        <v>5</v>
+      </c>
+      <c r="W706" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="707" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A707" s="15">
+        <v>753</v>
+      </c>
+      <c r="B707" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C707" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D707" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E707" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F707" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G707" s="15">
+        <v>20</v>
+      </c>
+      <c r="H707" s="15">
+        <v>22</v>
+      </c>
+      <c r="I707" s="15">
+        <v>20</v>
+      </c>
+      <c r="J707" s="15">
+        <v>35</v>
+      </c>
+      <c r="K707" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L707" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N707" s="15">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="O707" s="15">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="P707" s="15">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Q707" s="15">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="R707" s="15">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="S707" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T707" s="15">
+        <v>15</v>
+      </c>
+      <c r="U707" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V707" s="15">
+        <v>5</v>
+      </c>
+      <c r="W707" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="708" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A708" s="15">
+        <v>754</v>
+      </c>
+      <c r="B708" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C708" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D708" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E708" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F708" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G708" s="15">
+        <v>30</v>
+      </c>
+      <c r="H708" s="15">
+        <v>22</v>
+      </c>
+      <c r="I708" s="15">
+        <v>20</v>
+      </c>
+      <c r="J708" s="15">
+        <v>35</v>
+      </c>
+      <c r="K708" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L708" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N708" s="15">
+        <v>1.08</v>
+      </c>
+      <c r="O708" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P708" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q708" s="15">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="R708" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S708" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T708" s="15">
+        <v>15</v>
+      </c>
+      <c r="U708" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V708" s="15">
+        <v>5</v>
+      </c>
+      <c r="W708" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="709" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A709" s="15">
+        <v>755</v>
+      </c>
+      <c r="B709" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C709" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D709" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E709" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F709" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G709" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H709" s="15">
+        <v>22</v>
+      </c>
+      <c r="I709" s="15">
+        <v>20</v>
+      </c>
+      <c r="J709" s="15">
+        <v>35</v>
+      </c>
+      <c r="K709" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L709" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N709" s="15">
+        <v>3.74</v>
+      </c>
+      <c r="O709" s="15">
+        <v>3.73</v>
+      </c>
+      <c r="P709" s="15">
+        <v>3.72</v>
+      </c>
+      <c r="Q709" s="15">
+        <v>3.73</v>
+      </c>
+      <c r="R709" s="15">
+        <v>3.73</v>
+      </c>
+      <c r="S709" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T709" s="15">
+        <v>15</v>
+      </c>
+      <c r="U709" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V709" s="15">
+        <v>5</v>
+      </c>
+      <c r="W709" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="710" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A710" s="15">
+        <v>756</v>
+      </c>
+      <c r="B710" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C710" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D710" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E710" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F710" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G710" s="15">
+        <v>20</v>
+      </c>
+      <c r="H710" s="15">
+        <v>22</v>
+      </c>
+      <c r="I710" s="15">
+        <v>20</v>
+      </c>
+      <c r="J710" s="15">
+        <v>35</v>
+      </c>
+      <c r="K710" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L710" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N710" s="15">
+        <v>5.03</v>
+      </c>
+      <c r="O710" s="15">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="P710" s="15">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="Q710" s="15">
+        <v>5.04</v>
+      </c>
+      <c r="R710" s="15">
+        <v>5.04</v>
+      </c>
+      <c r="S710" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T710" s="15">
+        <v>15</v>
+      </c>
+      <c r="U710" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V710" s="15">
+        <v>5</v>
+      </c>
+      <c r="W710" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="711" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A711" s="15">
+        <v>757</v>
+      </c>
+      <c r="B711" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C711" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D711" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E711" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F711" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G711" s="15">
+        <v>30</v>
+      </c>
+      <c r="H711" s="15">
+        <v>22</v>
+      </c>
+      <c r="I711" s="15">
+        <v>20</v>
+      </c>
+      <c r="J711" s="15">
+        <v>35</v>
+      </c>
+      <c r="K711" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L711" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N711" s="15">
+        <v>6.5</v>
+      </c>
+      <c r="O711" s="15">
+        <v>6.45</v>
+      </c>
+      <c r="P711" s="15">
+        <v>6.46</v>
+      </c>
+      <c r="Q711" s="15">
+        <v>6.44</v>
+      </c>
+      <c r="R711" s="15">
+        <v>6.46</v>
+      </c>
+      <c r="S711" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T711" s="15">
+        <v>15</v>
+      </c>
+      <c r="U711" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V711" s="15">
+        <v>5</v>
+      </c>
+      <c r="W711" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="712" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A712" s="15">
+        <v>758</v>
+      </c>
+      <c r="B712" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C712" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D712" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E712" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F712" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G712" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H712" s="15">
+        <v>22</v>
+      </c>
+      <c r="I712" s="15">
+        <v>20</v>
+      </c>
+      <c r="J712" s="15">
+        <v>35</v>
+      </c>
+      <c r="K712" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L712" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N712" s="15">
+        <v>6</v>
+      </c>
+      <c r="O712" s="15">
+        <v>6.01</v>
+      </c>
+      <c r="P712" s="15">
+        <v>6.01</v>
+      </c>
+      <c r="Q712" s="15">
+        <v>6.02</v>
+      </c>
+      <c r="R712" s="15">
+        <v>6.01</v>
+      </c>
+      <c r="S712" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T712" s="15">
+        <v>15</v>
+      </c>
+      <c r="U712" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V712" s="15">
+        <v>5</v>
+      </c>
+      <c r="W712" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="713" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A713" s="15">
+        <v>759</v>
+      </c>
+      <c r="B713" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C713" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D713" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E713" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F713" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G713" s="15">
+        <v>20</v>
+      </c>
+      <c r="H713" s="15">
+        <v>22</v>
+      </c>
+      <c r="I713" s="15">
+        <v>20</v>
+      </c>
+      <c r="J713" s="15">
+        <v>35</v>
+      </c>
+      <c r="K713" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L713" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N713" s="15">
+        <v>7.04</v>
+      </c>
+      <c r="O713" s="15">
+        <v>7.05</v>
+      </c>
+      <c r="P713" s="15">
+        <v>7.03</v>
+      </c>
+      <c r="Q713" s="15">
+        <v>7.01</v>
+      </c>
+      <c r="R713" s="15">
+        <v>7.03</v>
+      </c>
+      <c r="S713" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T713" s="15">
+        <v>15</v>
+      </c>
+      <c r="U713" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V713" s="15">
+        <v>5</v>
+      </c>
+      <c r="W713" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="714" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A714" s="15">
+        <v>760</v>
+      </c>
+      <c r="B714" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C714" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D714" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E714" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F714" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G714" s="15">
+        <v>30</v>
+      </c>
+      <c r="H714" s="15">
+        <v>22</v>
+      </c>
+      <c r="I714" s="15">
+        <v>20</v>
+      </c>
+      <c r="J714" s="15">
+        <v>35</v>
+      </c>
+      <c r="K714" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L714" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N714" s="15">
+        <v>7.27</v>
+      </c>
+      <c r="O714" s="15">
+        <v>7.27</v>
+      </c>
+      <c r="P714" s="15">
+        <v>7.25</v>
+      </c>
+      <c r="Q714" s="15">
+        <v>7.25</v>
+      </c>
+      <c r="R714" s="15">
+        <v>7.26</v>
+      </c>
+      <c r="S714" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T714" s="15">
+        <v>15</v>
+      </c>
+      <c r="U714" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V714" s="15">
+        <v>5</v>
+      </c>
+      <c r="W714" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="715" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A715" s="15">
+        <v>761</v>
+      </c>
+      <c r="B715" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C715" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D715" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E715" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F715" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G715" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H715" s="15">
+        <v>22</v>
+      </c>
+      <c r="I715" s="15">
+        <v>20</v>
+      </c>
+      <c r="J715" s="15">
+        <v>35</v>
+      </c>
+      <c r="K715" s="15">
+        <v>4</v>
+      </c>
+      <c r="L715" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N715" s="15">
+        <v>6.48</v>
+      </c>
+      <c r="O715" s="15">
+        <v>6.52</v>
+      </c>
+      <c r="P715" s="15">
+        <v>6.48</v>
+      </c>
+      <c r="Q715" s="15">
+        <v>6.52</v>
+      </c>
+      <c r="R715" s="15">
+        <v>6.5</v>
+      </c>
+      <c r="S715" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T715" s="15">
+        <v>15</v>
+      </c>
+      <c r="U715" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V715" s="15">
+        <v>5</v>
+      </c>
+      <c r="W715" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="716" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A716" s="15">
+        <v>762</v>
+      </c>
+      <c r="B716" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C716" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D716" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E716" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F716" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G716" s="15">
+        <v>20</v>
+      </c>
+      <c r="H716" s="15">
+        <v>22</v>
+      </c>
+      <c r="I716" s="15">
+        <v>20</v>
+      </c>
+      <c r="J716" s="15">
+        <v>35</v>
+      </c>
+      <c r="K716" s="15">
+        <v>4</v>
+      </c>
+      <c r="L716" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N716" s="15">
+        <v>7.01</v>
+      </c>
+      <c r="O716" s="15">
+        <v>7.01</v>
+      </c>
+      <c r="P716" s="15">
+        <v>7</v>
+      </c>
+      <c r="Q716" s="15">
+        <v>7.02</v>
+      </c>
+      <c r="R716" s="15">
+        <v>7.01</v>
+      </c>
+      <c r="S716" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T716" s="15">
+        <v>15</v>
+      </c>
+      <c r="U716" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V716" s="15">
+        <v>5</v>
+      </c>
+      <c r="W716" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="717" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A717" s="15">
+        <v>763</v>
+      </c>
+      <c r="B717" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C717" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D717" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E717" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F717" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G717" s="15">
+        <v>30</v>
+      </c>
+      <c r="H717" s="15">
+        <v>22</v>
+      </c>
+      <c r="I717" s="15">
+        <v>20</v>
+      </c>
+      <c r="J717" s="15">
+        <v>35</v>
+      </c>
+      <c r="K717" s="15">
+        <v>4</v>
+      </c>
+      <c r="L717" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N717" s="15">
+        <v>6.62</v>
+      </c>
+      <c r="O717" s="15">
+        <v>6.63</v>
+      </c>
+      <c r="P717" s="15">
+        <v>6.66</v>
+      </c>
+      <c r="Q717" s="15">
+        <v>6.64</v>
+      </c>
+      <c r="R717" s="15">
+        <v>6.64</v>
+      </c>
+      <c r="S717" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T717" s="15">
+        <v>15</v>
+      </c>
+      <c r="U717" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V717" s="15">
+        <v>5</v>
+      </c>
+      <c r="W717" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="718" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A718" s="15">
+        <v>764</v>
+      </c>
+      <c r="B718" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C718" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D718" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E718" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F718" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G718" s="15">
+        <v>10</v>
+      </c>
+      <c r="H718" s="15">
+        <v>22</v>
+      </c>
+      <c r="I718" s="15">
+        <v>20</v>
+      </c>
+      <c r="J718" s="15">
+        <v>25</v>
+      </c>
+      <c r="K718" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L718" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N718" s="15">
+        <v>0.19</v>
+      </c>
+      <c r="O718" s="15">
+        <v>0.21</v>
+      </c>
+      <c r="P718" s="15">
+        <v>0.21</v>
+      </c>
+      <c r="Q718" s="15">
+        <v>0.21</v>
+      </c>
+      <c r="R718" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="S718" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T718" s="15">
+        <v>15</v>
+      </c>
+      <c r="U718" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V718" s="15">
+        <v>5</v>
+      </c>
+      <c r="W718" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="719" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A719" s="15">
+        <v>765</v>
+      </c>
+      <c r="B719" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C719" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D719" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E719" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F719" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G719" s="15">
+        <v>10</v>
+      </c>
+      <c r="H719" s="15">
+        <v>22</v>
+      </c>
+      <c r="I719" s="15">
+        <v>20</v>
+      </c>
+      <c r="J719" s="15">
+        <v>25</v>
+      </c>
+      <c r="K719" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L719" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N719" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="O719" s="15">
+        <v>1.46</v>
+      </c>
+      <c r="P719" s="15">
+        <v>1.47</v>
+      </c>
+      <c r="Q719" s="15">
+        <v>1.46</v>
+      </c>
+      <c r="R719" s="15">
+        <v>1.46</v>
+      </c>
+      <c r="S719" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T719" s="15">
+        <v>15</v>
+      </c>
+      <c r="U719" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V719" s="15">
+        <v>5</v>
+      </c>
+      <c r="W719" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="720" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A720" s="15">
+        <v>766</v>
+      </c>
+      <c r="B720" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C720" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D720" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E720" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F720" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G720" s="15">
+        <v>10</v>
+      </c>
+      <c r="H720" s="15">
+        <v>22</v>
+      </c>
+      <c r="I720" s="15">
+        <v>20</v>
+      </c>
+      <c r="J720" s="15">
+        <v>25</v>
+      </c>
+      <c r="K720" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L720" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N720" s="15">
+        <v>3.25</v>
+      </c>
+      <c r="O720" s="15">
+        <v>3.27</v>
+      </c>
+      <c r="P720" s="15">
+        <v>3.27</v>
+      </c>
+      <c r="Q720" s="15">
+        <v>3.28</v>
+      </c>
+      <c r="R720" s="15">
+        <v>3.27</v>
+      </c>
+      <c r="S720" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T720" s="15">
+        <v>15</v>
+      </c>
+      <c r="U720" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V720" s="15">
+        <v>5</v>
+      </c>
+      <c r="W720" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="721" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A721" s="15">
+        <v>767</v>
+      </c>
+      <c r="B721" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C721" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D721" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E721" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F721" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G721" s="15">
+        <v>10</v>
+      </c>
+      <c r="H721" s="15">
+        <v>22</v>
+      </c>
+      <c r="I721" s="15">
+        <v>20</v>
+      </c>
+      <c r="J721" s="15">
+        <v>25</v>
+      </c>
+      <c r="K721" s="15">
+        <v>4</v>
+      </c>
+      <c r="L721" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N721" s="15">
+        <v>3.65</v>
+      </c>
+      <c r="O721" s="15">
+        <v>3.63</v>
+      </c>
+      <c r="P721" s="15">
+        <v>3.66</v>
+      </c>
+      <c r="Q721" s="15">
+        <v>3.63</v>
+      </c>
+      <c r="R721" s="15">
+        <v>3.64</v>
+      </c>
+      <c r="S721" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T721" s="15">
+        <v>15</v>
+      </c>
+      <c r="U721" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V721" s="15">
+        <v>5</v>
+      </c>
+      <c r="W721" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="722" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A722" s="15">
+        <v>768</v>
+      </c>
+      <c r="B722" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C722" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D722" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E722" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F722" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G722" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H722" s="15">
+        <v>22</v>
+      </c>
+      <c r="I722" s="15">
+        <v>20</v>
+      </c>
+      <c r="J722" s="15">
+        <v>25</v>
+      </c>
+      <c r="K722" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L722" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N722" s="15">
+        <v>0.19</v>
+      </c>
+      <c r="O722" s="15">
+        <v>0.21</v>
+      </c>
+      <c r="P722" s="15">
+        <v>0.21</v>
+      </c>
+      <c r="Q722" s="15">
+        <v>0.21</v>
+      </c>
+      <c r="R722" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="S722" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T722" s="15">
+        <v>15</v>
+      </c>
+      <c r="U722" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V722" s="15">
+        <v>5</v>
+      </c>
+      <c r="W722" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="723" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A723" s="15">
+        <v>769</v>
+      </c>
+      <c r="B723" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C723" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D723" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E723" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F723" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G723" s="15">
+        <v>20</v>
+      </c>
+      <c r="H723" s="15">
+        <v>22</v>
+      </c>
+      <c r="I723" s="15">
+        <v>20</v>
+      </c>
+      <c r="J723" s="15">
+        <v>25</v>
+      </c>
+      <c r="K723" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L723" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N723" s="15">
+        <v>0.19</v>
+      </c>
+      <c r="O723" s="15">
+        <v>0.19</v>
+      </c>
+      <c r="P723" s="15">
+        <v>0.19</v>
+      </c>
+      <c r="Q723" s="15">
+        <v>0.19</v>
+      </c>
+      <c r="R723" s="15">
+        <v>0.19</v>
+      </c>
+      <c r="S723" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T723" s="15">
+        <v>15</v>
+      </c>
+      <c r="U723" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V723" s="15">
+        <v>5</v>
+      </c>
+      <c r="W723" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="724" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A724" s="15">
+        <v>770</v>
+      </c>
+      <c r="B724" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C724" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D724" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E724" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F724" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G724" s="15">
+        <v>30</v>
+      </c>
+      <c r="H724" s="15">
+        <v>22</v>
+      </c>
+      <c r="I724" s="15">
+        <v>20</v>
+      </c>
+      <c r="J724" s="15">
+        <v>25</v>
+      </c>
+      <c r="K724" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L724" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N724" s="15">
+        <v>0.16</v>
+      </c>
+      <c r="O724" s="15">
+        <v>0.16</v>
+      </c>
+      <c r="P724" s="15">
+        <v>0.16</v>
+      </c>
+      <c r="Q724" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="R724" s="15">
+        <v>0.16</v>
+      </c>
+      <c r="S724" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T724" s="15">
+        <v>15</v>
+      </c>
+      <c r="U724" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V724" s="15">
+        <v>5</v>
+      </c>
+      <c r="W724" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="725" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A725" s="15">
+        <v>771</v>
+      </c>
+      <c r="B725" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C725" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D725" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E725" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F725" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G725" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H725" s="15">
+        <v>22</v>
+      </c>
+      <c r="I725" s="15">
+        <v>20</v>
+      </c>
+      <c r="J725" s="15">
+        <v>25</v>
+      </c>
+      <c r="K725" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L725" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N725" s="15">
+        <v>1.74</v>
+      </c>
+      <c r="O725" s="15">
+        <v>1.74</v>
+      </c>
+      <c r="P725" s="15">
+        <v>1.74</v>
+      </c>
+      <c r="Q725" s="15">
+        <v>1.76</v>
+      </c>
+      <c r="R725" s="15">
+        <v>1.75</v>
+      </c>
+      <c r="S725" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T725" s="15">
+        <v>15</v>
+      </c>
+      <c r="U725" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V725" s="15">
+        <v>5</v>
+      </c>
+      <c r="W725" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="726" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A726" s="15">
+        <v>772</v>
+      </c>
+      <c r="B726" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C726" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D726" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E726" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F726" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G726" s="15">
+        <v>20</v>
+      </c>
+      <c r="H726" s="15">
+        <v>22</v>
+      </c>
+      <c r="I726" s="15">
+        <v>20</v>
+      </c>
+      <c r="J726" s="15">
+        <v>25</v>
+      </c>
+      <c r="K726" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L726" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N726" s="15">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="O726" s="15">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="P726" s="15">
+        <v>2.19</v>
+      </c>
+      <c r="Q726" s="15">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="R726" s="15">
+        <v>2.21</v>
+      </c>
+      <c r="S726" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T726" s="15">
+        <v>15</v>
+      </c>
+      <c r="U726" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V726" s="15">
+        <v>5</v>
+      </c>
+      <c r="W726" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="727" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A727" s="15">
+        <v>773</v>
+      </c>
+      <c r="B727" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C727" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D727" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E727" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F727" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G727" s="15">
+        <v>30</v>
+      </c>
+      <c r="H727" s="15">
+        <v>22</v>
+      </c>
+      <c r="I727" s="15">
+        <v>20</v>
+      </c>
+      <c r="J727" s="15">
+        <v>25</v>
+      </c>
+      <c r="K727" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L727" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N727" s="15">
+        <v>2.68</v>
+      </c>
+      <c r="O727" s="15">
+        <v>2.68</v>
+      </c>
+      <c r="P727" s="15">
+        <v>2.69</v>
+      </c>
+      <c r="Q727" s="15">
+        <v>2.69</v>
+      </c>
+      <c r="R727" s="15">
+        <v>2.69</v>
+      </c>
+      <c r="S727" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T727" s="15">
+        <v>15</v>
+      </c>
+      <c r="U727" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V727" s="15">
+        <v>5</v>
+      </c>
+      <c r="W727" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="728" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A728" s="15">
+        <v>774</v>
+      </c>
+      <c r="B728" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C728" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D728" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E728" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F728" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G728" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H728" s="15">
+        <v>22</v>
+      </c>
+      <c r="I728" s="15">
+        <v>20</v>
+      </c>
+      <c r="J728" s="15">
+        <v>25</v>
+      </c>
+      <c r="K728" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L728" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N728" s="15">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="O728" s="15">
+        <v>4.04</v>
+      </c>
+      <c r="P728" s="15">
+        <v>4.03</v>
+      </c>
+      <c r="Q728" s="15">
+        <v>4.03</v>
+      </c>
+      <c r="R728" s="15">
+        <v>4.03</v>
+      </c>
+      <c r="S728" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T728" s="15">
+        <v>15</v>
+      </c>
+      <c r="U728" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V728" s="15">
+        <v>5</v>
+      </c>
+      <c r="W728" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="729" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A729" s="15">
+        <v>775</v>
+      </c>
+      <c r="B729" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C729" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D729" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E729" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F729" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G729" s="15">
+        <v>20</v>
+      </c>
+      <c r="H729" s="15">
+        <v>22</v>
+      </c>
+      <c r="I729" s="15">
+        <v>20</v>
+      </c>
+      <c r="J729" s="15">
+        <v>25</v>
+      </c>
+      <c r="K729" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L729" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N729" s="15">
+        <v>5.25</v>
+      </c>
+      <c r="O729" s="15">
+        <v>5.24</v>
+      </c>
+      <c r="P729" s="15">
+        <v>5.25</v>
+      </c>
+      <c r="Q729" s="15">
+        <v>5.26</v>
+      </c>
+      <c r="R729" s="15">
+        <v>5.25</v>
+      </c>
+      <c r="S729" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T729" s="15">
+        <v>15</v>
+      </c>
+      <c r="U729" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V729" s="15">
+        <v>5</v>
+      </c>
+      <c r="W729" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="730" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A730" s="15">
+        <v>776</v>
+      </c>
+      <c r="B730" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C730" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D730" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E730" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F730" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G730" s="15">
+        <v>30</v>
+      </c>
+      <c r="H730" s="15">
+        <v>22</v>
+      </c>
+      <c r="I730" s="15">
+        <v>20</v>
+      </c>
+      <c r="J730" s="15">
+        <v>25</v>
+      </c>
+      <c r="K730" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L730" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N730" s="15">
+        <v>6.31</v>
+      </c>
+      <c r="O730" s="15">
+        <v>6.33</v>
+      </c>
+      <c r="P730" s="15">
+        <v>6.33</v>
+      </c>
+      <c r="Q730" s="15">
+        <v>6.32</v>
+      </c>
+      <c r="R730" s="15">
+        <v>6.32</v>
+      </c>
+      <c r="S730" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T730" s="15">
+        <v>15</v>
+      </c>
+      <c r="U730" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V730" s="15">
+        <v>5</v>
+      </c>
+      <c r="W730" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="731" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A731" s="15">
+        <v>777</v>
+      </c>
+      <c r="B731" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C731" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D731" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E731" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F731" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G731" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H731" s="15">
+        <v>22</v>
+      </c>
+      <c r="I731" s="15">
+        <v>20</v>
+      </c>
+      <c r="J731" s="15">
+        <v>25</v>
+      </c>
+      <c r="K731" s="15">
+        <v>4</v>
+      </c>
+      <c r="L731" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N731" s="15">
+        <v>4.59</v>
+      </c>
+      <c r="O731" s="15">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="P731" s="15">
+        <v>4.59</v>
+      </c>
+      <c r="Q731" s="15">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R731" s="15">
+        <v>4.59</v>
+      </c>
+      <c r="S731" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T731" s="15">
+        <v>15</v>
+      </c>
+      <c r="U731" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V731" s="15">
+        <v>5</v>
+      </c>
+      <c r="W731" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="732" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A732" s="15">
+        <v>778</v>
+      </c>
+      <c r="B732" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C732" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D732" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E732" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F732" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G732" s="15">
+        <v>20</v>
+      </c>
+      <c r="H732" s="15">
+        <v>22</v>
+      </c>
+      <c r="I732" s="15">
+        <v>20</v>
+      </c>
+      <c r="J732" s="15">
+        <v>25</v>
+      </c>
+      <c r="K732" s="15">
+        <v>4</v>
+      </c>
+      <c r="L732" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N732" s="15">
+        <v>5.67</v>
+      </c>
+      <c r="O732" s="15">
+        <v>5.65</v>
+      </c>
+      <c r="P732" s="15">
+        <v>5.65</v>
+      </c>
+      <c r="Q732" s="15">
+        <v>5.68</v>
+      </c>
+      <c r="R732" s="15">
+        <v>5.66</v>
+      </c>
+      <c r="S732" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T732" s="15">
+        <v>15</v>
+      </c>
+      <c r="U732" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V732" s="15">
+        <v>5</v>
+      </c>
+      <c r="W732" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="733" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A733" s="15">
+        <v>779</v>
+      </c>
+      <c r="B733" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C733" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D733" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E733" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F733" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G733" s="15">
+        <v>30</v>
+      </c>
+      <c r="H733" s="15">
+        <v>22</v>
+      </c>
+      <c r="I733" s="15">
+        <v>20</v>
+      </c>
+      <c r="J733" s="15">
+        <v>25</v>
+      </c>
+      <c r="K733" s="15">
+        <v>4</v>
+      </c>
+      <c r="L733" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N733" s="15">
+        <v>6.39</v>
+      </c>
+      <c r="O733" s="15">
+        <v>6.35</v>
+      </c>
+      <c r="P733" s="15">
+        <v>6.35</v>
+      </c>
+      <c r="Q733" s="15">
+        <v>6.38</v>
+      </c>
+      <c r="R733" s="15">
+        <v>6.37</v>
+      </c>
+      <c r="S733" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T733" s="15">
+        <v>15</v>
+      </c>
+      <c r="U733" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V733" s="15">
+        <v>5</v>
+      </c>
+      <c r="W733" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="734" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A734" s="15">
+        <v>780</v>
+      </c>
+      <c r="B734" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C734" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D734" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E734" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F734" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G734" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H734" s="15">
+        <v>22</v>
+      </c>
+      <c r="I734" s="15">
+        <v>20</v>
+      </c>
+      <c r="J734" s="15">
+        <v>60</v>
+      </c>
+      <c r="K734" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L734" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N734" s="15">
+        <v>3.34</v>
+      </c>
+      <c r="O734" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="P734" s="15">
+        <v>3.43</v>
+      </c>
+      <c r="Q734" s="15">
+        <v>3.45</v>
+      </c>
+      <c r="R734" s="15">
+        <v>3.41</v>
+      </c>
+      <c r="S734" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T734" s="15">
+        <v>15</v>
+      </c>
+      <c r="U734" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V734" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="735" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A735" s="15">
+        <v>781</v>
+      </c>
+      <c r="B735" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C735" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D735" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E735" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F735" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G735" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H735" s="15">
+        <v>22</v>
+      </c>
+      <c r="I735" s="15">
+        <v>20</v>
+      </c>
+      <c r="J735" s="15">
+        <v>60</v>
+      </c>
+      <c r="K735" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="L735" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N735" s="15">
+        <v>12.87</v>
+      </c>
+      <c r="O735" s="15">
+        <v>12.94</v>
+      </c>
+      <c r="P735" s="15">
+        <v>12.88</v>
+      </c>
+      <c r="Q735" s="15">
+        <v>12.95</v>
+      </c>
+      <c r="R735" s="15">
+        <v>12.91</v>
+      </c>
+      <c r="S735" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T735" s="15">
+        <v>15</v>
+      </c>
+      <c r="U735" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V735" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="736" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A736" s="15">
+        <v>782</v>
+      </c>
+      <c r="B736" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C736" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D736" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E736" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F736" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G736" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H736" s="15">
+        <v>22</v>
+      </c>
+      <c r="I736" s="15">
+        <v>20</v>
+      </c>
+      <c r="J736" s="15">
+        <v>60</v>
+      </c>
+      <c r="K736" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="L736" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N736" s="15">
+        <v>14.98</v>
+      </c>
+      <c r="O736" s="15">
+        <v>15.01</v>
+      </c>
+      <c r="P736" s="15">
+        <v>15.02</v>
+      </c>
+      <c r="Q736" s="15">
+        <v>15.04</v>
+      </c>
+      <c r="R736" s="15">
+        <v>15.01</v>
+      </c>
+      <c r="S736" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T736" s="15">
+        <v>15</v>
+      </c>
+      <c r="U736" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V736" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="737" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A737" s="15">
+        <v>783</v>
+      </c>
+      <c r="B737" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C737" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D737" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E737" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F737" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G737" s="15">
+        <v>12.5</v>
+      </c>
+      <c r="H737" s="15">
+        <v>22</v>
+      </c>
+      <c r="I737" s="15">
+        <v>20</v>
+      </c>
+      <c r="J737" s="15">
+        <v>60</v>
+      </c>
+      <c r="K737" s="15">
+        <v>4</v>
+      </c>
+      <c r="L737" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N737" s="15">
+        <v>14.53</v>
+      </c>
+      <c r="O737" s="15">
+        <v>14.53</v>
+      </c>
+      <c r="P737" s="15">
+        <v>14.57</v>
+      </c>
+      <c r="Q737" s="15">
+        <v>14.51</v>
+      </c>
+      <c r="R737" s="15">
+        <v>14.54</v>
+      </c>
+      <c r="S737" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="T737" s="15">
+        <v>15</v>
+      </c>
+      <c r="U737" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="V737" s="15">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>